<commit_message>
Arbeitstagebuch vom 11.12.23 aktualisiert und erweitert
</commit_message>
<xml_diff>
--- a/Dokumentation/Projekt-Steuerung_Autonom-Fahrendes-Auto_Gruppe_4.xlsx
+++ b/Dokumentation/Projekt-Steuerung_Autonom-Fahrendes-Auto_Gruppe_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\esy\projekt\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697684F7-CF9F-4079-8918-5F109913A11C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023650D0-CF8D-404B-A380-D5F63CB6F481}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7515" tabRatio="752" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7515" tabRatio="752" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -1132,7 +1132,7 @@
     <t>Sourcetree installiert</t>
   </si>
   <si>
-    <t>Sensoren programmiert jedoch zu keinem wertvollen Ergebnis gekommen</t>
+    <t>Sensoren programmiert jedoch zu keinem wertvollen Ergebnis gekommen, analogread verwendet zum einlesen des signals&gt; kein Erfolg, Sensoren werden nicht richtig angesteuert</t>
   </si>
 </sst>
 </file>
@@ -1915,6 +1915,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1933,32 +1957,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2469,14 +2469,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="118" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2525,10 +2525,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="124" t="s">
+      <c r="E7" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="124"/>
+      <c r="F7" s="119"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2539,8 +2539,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="130"/>
-      <c r="F8" s="130"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2551,8 +2551,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2563,8 +2563,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2575,8 +2575,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2597,49 +2597,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="127"/>
-      <c r="C15" s="127"/>
-      <c r="D15" s="127"/>
-      <c r="E15" s="127"/>
-      <c r="F15" s="127"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="128"/>
-      <c r="C16" s="128"/>
-      <c r="D16" s="128"/>
-      <c r="E16" s="128"/>
-      <c r="F16" s="128"/>
+      <c r="B16" s="125"/>
+      <c r="C16" s="125"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="125"/>
+      <c r="F16" s="125"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="128"/>
-      <c r="C17" s="128"/>
-      <c r="D17" s="128"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="128"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="125"/>
+      <c r="F17" s="125"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="128"/>
-      <c r="C18" s="128"/>
-      <c r="D18" s="128"/>
-      <c r="E18" s="128"/>
-      <c r="F18" s="128"/>
+      <c r="B18" s="125"/>
+      <c r="C18" s="125"/>
+      <c r="D18" s="125"/>
+      <c r="E18" s="125"/>
+      <c r="F18" s="125"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="122"/>
+      <c r="B19" s="130"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="130"/>
+      <c r="E19" s="130"/>
+      <c r="F19" s="130"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2652,74 +2652,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="131"/>
+      <c r="D23" s="131"/>
+      <c r="E23" s="131"/>
+      <c r="F23" s="131"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="124" t="s">
+      <c r="A26" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="124"/>
-      <c r="C26" s="124"/>
-      <c r="D26" s="124" t="s">
+      <c r="B26" s="119"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="124"/>
-      <c r="F26" s="124"/>
+      <c r="E26" s="119"/>
+      <c r="F26" s="119"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="119" t="s">
+      <c r="A27" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="119"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="125"/>
-      <c r="E27" s="125"/>
-      <c r="F27" s="125"/>
+      <c r="B27" s="127"/>
+      <c r="C27" s="127"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="132"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="118" t="s">
+      <c r="A28" s="126" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="119" t="s">
+      <c r="B28" s="126"/>
+      <c r="C28" s="126"/>
+      <c r="D28" s="127" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
+      <c r="E28" s="127"/>
+      <c r="F28" s="127"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="120" t="s">
+      <c r="A29" s="128" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="120"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
+      <c r="B29" s="128"/>
+      <c r="C29" s="128"/>
+      <c r="D29" s="129"/>
+      <c r="E29" s="129"/>
+      <c r="F29" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2730,6 +2720,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2744,8 +2744,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2873,7 +2873,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>45267</v>
       </c>
@@ -3059,11 +3059,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="133" t="s">
@@ -3897,16 +3897,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -6091,8 +6091,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6231,7 +6231,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>45267</v>
       </c>

</xml_diff>

<commit_message>
08.01.2024 aktuallisiert Dokumentation und Code
</commit_message>
<xml_diff>
--- a/Dokumentation/Projekt-Steuerung_Autonom-Fahrendes-Auto_Gruppe_4.xlsx
+++ b/Dokumentation/Projekt-Steuerung_Autonom-Fahrendes-Auto_Gruppe_4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\esy\projekt\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\001152\Documents\group-04\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562736B2-28DD-4CC5-8511-2C0777944BFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2035B51F-5547-4EA7-86F4-44E1FBAE93BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7515" tabRatio="752" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7515" tabRatio="752" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="235">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1136,6 +1136,12 @@
   </si>
   <si>
     <t>An Sensoren gearbeitet, Auf etwas gestoßen, gemerkt, dass man einen Kehrwert bilden muss damit richtige Werte angezeigt werden am Serial Monitor. Geradengleichung mit Herr Professor aufgestellt.</t>
+  </si>
+  <si>
+    <t>Sensoren abgebaut und überlegt wo man sie einbauen kann</t>
+  </si>
+  <si>
+    <t>Sensoren verstehen um es einzusetzen ( Wir verwenden Sensor Werte )</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1579,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1913,6 +1919,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3421,14 +3430,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -3477,10 +3486,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="125" t="s">
+      <c r="E7" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="125"/>
+      <c r="F7" s="126"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -3491,8 +3500,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -3503,8 +3512,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -3515,8 +3524,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
+      <c r="E10" s="134"/>
+      <c r="F10" s="134"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -3527,8 +3536,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="127"/>
-      <c r="F11" s="127"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="128"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -3549,49 +3558,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="128"/>
-      <c r="C15" s="128"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
-      <c r="F15" s="128"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="129"/>
+      <c r="D15" s="129"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="129"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="129"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="129"/>
-      <c r="E16" s="129"/>
-      <c r="F16" s="129"/>
+      <c r="B16" s="130"/>
+      <c r="C16" s="130"/>
+      <c r="D16" s="130"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="130"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="129"/>
-      <c r="C17" s="129"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="129"/>
-      <c r="F17" s="129"/>
+      <c r="B17" s="130"/>
+      <c r="C17" s="130"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="130"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="129"/>
-      <c r="C18" s="129"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="129"/>
-      <c r="F18" s="129"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="123"/>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="123"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="124"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -3604,61 +3613,61 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="124" t="s">
+      <c r="A23" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="124"/>
-      <c r="C23" s="124"/>
-      <c r="D23" s="124"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="124"/>
+      <c r="B23" s="125"/>
+      <c r="C23" s="125"/>
+      <c r="D23" s="125"/>
+      <c r="E23" s="125"/>
+      <c r="F23" s="125"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="125" t="s">
+      <c r="A26" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="125"/>
-      <c r="C26" s="125"/>
-      <c r="D26" s="125" t="s">
+      <c r="B26" s="126"/>
+      <c r="C26" s="126"/>
+      <c r="D26" s="126" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="125"/>
-      <c r="F26" s="125"/>
+      <c r="E26" s="126"/>
+      <c r="F26" s="126"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="120" t="s">
+      <c r="A27" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="120"/>
-      <c r="C27" s="120"/>
-      <c r="D27" s="126"/>
-      <c r="E27" s="126"/>
-      <c r="F27" s="126"/>
+      <c r="B27" s="121"/>
+      <c r="C27" s="121"/>
+      <c r="D27" s="127"/>
+      <c r="E27" s="127"/>
+      <c r="F27" s="127"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="119"/>
-      <c r="C28" s="119"/>
-      <c r="D28" s="120" t="s">
+      <c r="B28" s="120"/>
+      <c r="C28" s="120"/>
+      <c r="D28" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="120"/>
-      <c r="F28" s="120"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="121" t="s">
+      <c r="A29" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="121"/>
-      <c r="C29" s="121"/>
-      <c r="D29" s="122"/>
-      <c r="E29" s="122"/>
-      <c r="F29" s="122"/>
+      <c r="B29" s="122"/>
+      <c r="C29" s="122"/>
+      <c r="D29" s="123"/>
+      <c r="E29" s="123"/>
+      <c r="F29" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -3696,8 +3705,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3709,11 +3718,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="136" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
     </row>
     <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3847,15 +3856,27 @@
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="2"/>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B15" s="41">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B16" s="41">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
@@ -4017,29 +4038,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="134" t="s">
+      <c r="B3" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="134"/>
+      <c r="C3" s="135"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="134" t="s">
+      <c r="B4" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="134"/>
+      <c r="C4" s="135"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="134" t="s">
+      <c r="B5" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="134"/>
+      <c r="C5" s="135"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -4248,10 +4269,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4262,11 +4283,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -4274,18 +4295,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="136"/>
-      <c r="C3" s="136"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="137" t="s">
+      <c r="A4" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="137"/>
-      <c r="C4" s="137"/>
+      <c r="B4" s="138"/>
+      <c r="C4" s="138"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -4332,7 +4353,9 @@
       <c r="B9" s="39">
         <v>45257</v>
       </c>
-      <c r="C9" s="39"/>
+      <c r="C9" s="39">
+        <v>45257</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -4353,9 +4376,7 @@
       <c r="C11" s="41"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="A12" s="119"/>
       <c r="B12" s="39">
         <v>45306</v>
       </c>
@@ -4363,7 +4384,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="39">
         <v>45320</v>
@@ -4372,25 +4393,25 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="39">
         <v>45341</v>
       </c>
       <c r="C14" s="41"/>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="39">
         <v>45355</v>
       </c>
       <c r="C15" s="41"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="39">
         <v>45362</v>
@@ -4398,17 +4419,21 @@
       <c r="C16" s="41"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="39">
+        <v>45362</v>
+      </c>
       <c r="C17" s="41"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="41"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="41"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -4418,12 +4443,12 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="40"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="41"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="41"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="41"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -4433,12 +4458,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="40"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="41"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -4517,9 +4542,14 @@
       <c r="C40" s="41"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="24"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4555,14 +4585,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="136" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4840,7 +4870,7 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -4855,16 +4885,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5487,19 +5517,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="139" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
@@ -6163,16 +6193,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="136" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -6948,71 +6978,71 @@
       <c r="A21" s="95" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="140" t="s">
+      <c r="B21" s="141" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="140"/>
-      <c r="D21" s="140"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="141"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="100" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="141" t="s">
+      <c r="B22" s="142" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="141"/>
-      <c r="D22" s="141"/>
+      <c r="C22" s="142"/>
+      <c r="D22" s="142"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="100" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="141" t="s">
+      <c r="B23" s="142" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="142"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="100" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="141" t="s">
+      <c r="B24" s="142" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="141"/>
-      <c r="D24" s="141"/>
+      <c r="C24" s="142"/>
+      <c r="D24" s="142"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="97"/>
-      <c r="B25" s="139"/>
-      <c r="C25" s="139"/>
-      <c r="D25" s="139"/>
+      <c r="B25" s="140"/>
+      <c r="C25" s="140"/>
+      <c r="D25" s="140"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="97"/>
-      <c r="B26" s="139"/>
-      <c r="C26" s="139"/>
-      <c r="D26" s="139"/>
+      <c r="B26" s="140"/>
+      <c r="C26" s="140"/>
+      <c r="D26" s="140"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="97"/>
-      <c r="B27" s="139"/>
-      <c r="C27" s="139"/>
-      <c r="D27" s="139"/>
+      <c r="B27" s="140"/>
+      <c r="C27" s="140"/>
+      <c r="D27" s="140"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="97"/>
-      <c r="B28" s="139"/>
-      <c r="C28" s="139"/>
-      <c r="D28" s="139"/>
+      <c r="B28" s="140"/>
+      <c r="C28" s="140"/>
+      <c r="D28" s="140"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="97"/>
-      <c r="B29" s="139"/>
-      <c r="C29" s="139"/>
-      <c r="D29" s="139"/>
+      <c r="B29" s="140"/>
+      <c r="C29" s="140"/>
+      <c r="D29" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -7062,11 +7092,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="136" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
     </row>
     <row r="3" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">

</xml_diff>

<commit_message>
Aktueller Stand der Dinge!!
</commit_message>
<xml_diff>
--- a/Dokumentation/Projekt-Steuerung_Autonom-Fahrendes-Auto_Gruppe_4.xlsx
+++ b/Dokumentation/Projekt-Steuerung_Autonom-Fahrendes-Auto_Gruppe_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\190040\Documents\group-04\Dokumentation\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946BC752-153F-48FB-855F-665A6A4A57CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B2E774-B1D7-4044-A7D2-9A6B30BB2057}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7515" tabRatio="752" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7515" tabRatio="752" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="246">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1169,6 +1169,12 @@
   </si>
   <si>
     <t>Loch in das Auto gebohrt um den dritten Sensor einzubauen. Danach mit Mustafic den Code erweitert mit den Codezeilen vom Herr Professor.</t>
+  </si>
+  <si>
+    <t>Dritten Sensor mit Heißkleber befestigt, dann dritten Sensor im Code implementiert mit Mustafic, vorderen Sensor neu verkabelt mit einem Stecker, ebenso paar Testfahrten gemacht und Auto hat es nicht geschafft bei der 2 Kurve zu lenken weil es zu schnell war.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dritten Sensor im Code implementiert mit Köklü, vorderen Sensor neu verkabelt mit einem Stecker, ebenso paar Testfahrten gemacht und Auto hat es nicht geschafft bei der 2 Kurve zu lenken weil es zu schnell war.</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1612,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1963,12 +1969,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1977,36 +2016,6 @@
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3463,14 +3472,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="134" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -3519,10 +3528,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="123" t="s">
+      <c r="E7" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="123"/>
+      <c r="F7" s="129"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -3533,8 +3542,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="124"/>
-      <c r="F8" s="124"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="135"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -3545,8 +3554,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="125"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -3557,8 +3566,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="126"/>
-      <c r="F10" s="126"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="137"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -3569,8 +3578,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="127"/>
-      <c r="F11" s="127"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -3591,49 +3600,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="128"/>
-      <c r="C15" s="128"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
-      <c r="F15" s="128"/>
+      <c r="B15" s="132"/>
+      <c r="C15" s="132"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="129"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="129"/>
-      <c r="E16" s="129"/>
-      <c r="F16" s="129"/>
+      <c r="B16" s="133"/>
+      <c r="C16" s="133"/>
+      <c r="D16" s="133"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="129"/>
-      <c r="C17" s="129"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="129"/>
-      <c r="F17" s="129"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="129"/>
-      <c r="C18" s="129"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="129"/>
-      <c r="F18" s="129"/>
+      <c r="B18" s="133"/>
+      <c r="C18" s="133"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="134"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="134"/>
-      <c r="F19" s="134"/>
+      <c r="B19" s="127"/>
+      <c r="C19" s="127"/>
+      <c r="D19" s="127"/>
+      <c r="E19" s="127"/>
+      <c r="F19" s="127"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -3646,64 +3655,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="135" t="s">
+      <c r="A23" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="135"/>
-      <c r="C23" s="135"/>
-      <c r="D23" s="135"/>
-      <c r="E23" s="135"/>
-      <c r="F23" s="135"/>
+      <c r="B23" s="128"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128"/>
+      <c r="F23" s="128"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="123" t="s">
+      <c r="A26" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="123"/>
-      <c r="C26" s="123"/>
-      <c r="D26" s="123" t="s">
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="123"/>
-      <c r="F26" s="123"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="129"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="131" t="s">
+      <c r="A27" s="124" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="131"/>
-      <c r="C27" s="131"/>
-      <c r="D27" s="136"/>
-      <c r="E27" s="136"/>
-      <c r="F27" s="136"/>
+      <c r="B27" s="124"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="130"/>
+      <c r="E27" s="130"/>
+      <c r="F27" s="130"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="130" t="s">
+      <c r="A28" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="130"/>
-      <c r="C28" s="130"/>
-      <c r="D28" s="131" t="s">
+      <c r="B28" s="123"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="124" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="131"/>
-      <c r="F28" s="131"/>
+      <c r="E28" s="124"/>
+      <c r="F28" s="124"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="132" t="s">
+      <c r="A29" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="132"/>
-      <c r="C29" s="132"/>
-      <c r="D29" s="133"/>
-      <c r="E29" s="133"/>
-      <c r="F29" s="133"/>
+      <c r="B29" s="125"/>
+      <c r="C29" s="125"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -3714,16 +3733,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3738,8 +3747,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3751,11 +3760,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="139" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
     </row>
     <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3955,10 +3964,16 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="2"/>
+    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="40">
+        <v>45369</v>
+      </c>
+      <c r="B21" s="41">
+        <v>2.5</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="41"/>
@@ -4095,29 +4110,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="137" t="s">
+      <c r="B3" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="137"/>
+      <c r="C3" s="138"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="137"/>
+      <c r="C4" s="138"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="137" t="s">
+      <c r="B5" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="137"/>
+      <c r="C5" s="138"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -4328,8 +4343,8 @@
   </sheetPr>
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4340,11 +4355,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="139" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -4352,18 +4367,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="139"/>
-      <c r="C3" s="139"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="140"/>
-      <c r="C4" s="140"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="141"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -4421,7 +4436,9 @@
       <c r="B10" s="40">
         <v>45271</v>
       </c>
-      <c r="C10" s="41"/>
+      <c r="C10" s="39">
+        <v>45369</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -4642,14 +4659,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="139" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4927,8 +4944,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4942,16 +4959,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="134" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5427,7 +5444,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27" s="64">
         <v>0</v>
@@ -5538,7 +5555,7 @@
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
@@ -5588,19 +5605,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="142" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
-      <c r="J1" s="141"/>
-      <c r="K1" s="141"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
@@ -6264,16 +6281,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="139" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -7049,71 +7066,71 @@
       <c r="A21" s="95" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="143" t="s">
+      <c r="B21" s="144" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="143"/>
-      <c r="D21" s="143"/>
+      <c r="C21" s="144"/>
+      <c r="D21" s="144"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="100" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="144" t="s">
+      <c r="B22" s="145" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="144"/>
-      <c r="D22" s="144"/>
+      <c r="C22" s="145"/>
+      <c r="D22" s="145"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="100" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="144" t="s">
+      <c r="B23" s="145" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
+      <c r="C23" s="145"/>
+      <c r="D23" s="145"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="100" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="144" t="s">
+      <c r="B24" s="145" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="144"/>
-      <c r="D24" s="144"/>
+      <c r="C24" s="145"/>
+      <c r="D24" s="145"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="97"/>
-      <c r="B25" s="142"/>
-      <c r="C25" s="142"/>
-      <c r="D25" s="142"/>
+      <c r="B25" s="143"/>
+      <c r="C25" s="143"/>
+      <c r="D25" s="143"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="97"/>
-      <c r="B26" s="142"/>
-      <c r="C26" s="142"/>
-      <c r="D26" s="142"/>
+      <c r="B26" s="143"/>
+      <c r="C26" s="143"/>
+      <c r="D26" s="143"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="97"/>
-      <c r="B27" s="142"/>
-      <c r="C27" s="142"/>
-      <c r="D27" s="142"/>
+      <c r="B27" s="143"/>
+      <c r="C27" s="143"/>
+      <c r="D27" s="143"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="97"/>
-      <c r="B28" s="142"/>
-      <c r="C28" s="142"/>
-      <c r="D28" s="142"/>
+      <c r="B28" s="143"/>
+      <c r="C28" s="143"/>
+      <c r="D28" s="143"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="97"/>
-      <c r="B29" s="142"/>
-      <c r="C29" s="142"/>
-      <c r="D29" s="142"/>
+      <c r="B29" s="143"/>
+      <c r="C29" s="143"/>
+      <c r="D29" s="143"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -7150,8 +7167,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:C21"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7163,11 +7180,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="139" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
     </row>
     <row r="3" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -7432,10 +7449,16 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="104"/>
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="40">
+        <v>45369</v>
+      </c>
+      <c r="B22" s="41">
+        <v>2.5</v>
+      </c>
+      <c r="C22" s="122" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>

</xml_diff>